<commit_message>
changes in data driven
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataDriven\NewFrameworkFromLinkedIn\automation-framework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAD948B-F7DB-4AA2-ABE0-EA72D47E1C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B03846-C125-4510-9BCD-8F6F0C878028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>fName</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>KrishE</t>
+  </si>
+  <si>
+    <t>UserOne</t>
+  </si>
+  <si>
+    <t>UserTwo</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,6 +397,17 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>35454</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>